<commit_message>
updated Decodon_hand_pollinations_2016 to include new columns for trays and collection
</commit_message>
<xml_diff>
--- a/Decodon_hand_pollinations_2016.xlsx
+++ b/Decodon_hand_pollinations_2016.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="27120" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="27120" windowHeight="16460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hand pollinations" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Set1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hand pollinations'!$A$1:$I$239</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Hand pollinations'!$A$1:$K$100</definedName>
   </definedNames>
   <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>within pop</t>
   </si>
@@ -41,9 +41,6 @@
     <t>self</t>
   </si>
   <si>
-    <t>Maternal Morph</t>
-  </si>
-  <si>
     <t>Maternal Flower Position</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>Maternal Pop</t>
   </si>
   <si>
-    <t>Paternal ID</t>
-  </si>
-  <si>
-    <t>Paternal Morph</t>
-  </si>
-  <si>
-    <t>Maternal ID</t>
-  </si>
-  <si>
     <t>ON.M6</t>
   </si>
   <si>
@@ -102,6 +90,24 @@
   </si>
   <si>
     <t>bd (between  pop but w diff type pop)</t>
+  </si>
+  <si>
+    <t>Collection date</t>
+  </si>
+  <si>
+    <t>Pat Morph</t>
+  </si>
+  <si>
+    <t>Mat Morph</t>
+  </si>
+  <si>
+    <t>Mat ID</t>
+  </si>
+  <si>
+    <t>Pat ID</t>
+  </si>
+  <si>
+    <t>Tray #</t>
   </si>
 </sst>
 </file>
@@ -411,7 +417,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -474,6 +480,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -757,155 +770,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="41" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="41" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="12" style="41" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="41" customWidth="1"/>
-    <col min="9" max="9" width="10" style="41" customWidth="1"/>
+    <col min="1" max="1" width="4" style="42" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="9" style="41" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="41" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="41" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="41" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="41" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="5" style="41" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="41" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>7</v>
+    <row r="1" spans="1:12" ht="85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>24</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="40" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K2" t="s">
+      <c r="K1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
+    <row r="3" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>22</v>
+    <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0" right="0" top="0.75" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="10"/>
+  <pageMargins left="0" right="0" top="0.75" bottom="0" header="0.05" footer="0.05"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="30"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="41" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="41" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="12" style="41" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="41" customWidth="1"/>
-    <col min="9" max="9" width="10" style="41" customWidth="1"/>
+    <col min="1" max="1" width="4" style="42" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="9" style="41" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="41" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="41" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="41" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="41" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="5" style="41" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="41" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>7</v>
+    <row r="1" spans="1:12" ht="85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>24</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="40" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K2" t="s">
+      <c r="K1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
+    <row r="3" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>22</v>
+    <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -931,112 +960,112 @@
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="24" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" s="29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1062,110 +1091,110 @@
     <row r="1" spans="1:6" ht="25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:6" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="F6" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="110" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>